<commit_message>
Added diagrams (sequence, class, statechart) Modified use case diagram
</commit_message>
<xml_diff>
--- a/Documentation/Glossary.xlsx
+++ b/Documentation/Glossary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Operand</t>
   </si>
   <si>
-    <t>Operand is a complex number which is part of calculation. There are two operands in application. In case of division, operand 1 is dividend and operand 2 is divident. In case of subtraction, operand 1 is subtractend and operand 2 is subtractor. (In cases of multiplication and addition, the operands operands oreder doesn't matter.)</t>
-  </si>
-  <si>
     <t>UI</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t>A group of fields that are representing numeric and exponential values of complex number that is the result of operation that was performed on operands. It is located on the top of application window. (See figure 2 in appendix A of requirements specification.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operand is a complex number which is part of calculation. </t>
   </si>
 </sst>
 </file>
@@ -505,14 +505,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="110.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -539,76 +539,76 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,8 +780,8 @@
       <c r="B54" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:B9">
-    <sortCondition ref="B9"/>
+  <sortState ref="A2:B12">
+    <sortCondition ref="B12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>